<commit_message>
fix : Adding User Data from Chrome to the Selenium
</commit_message>
<xml_diff>
--- a/coba.xlsx
+++ b/coba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\99 - MLPT SportsClub\dockerized\auto-fill-ms-form\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RnD\auto-fill-ms-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CEE432-083E-4BD4-8D14-3AD3A572F540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5FEB69-F476-4021-8F1F-8406759BE4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>NIK</t>
   </si>
@@ -33,46 +33,28 @@
     <t>NAMA</t>
   </si>
   <si>
+    <t>Adam Kurniawan Takariyanto</t>
+  </si>
+  <si>
+    <t>Hendro Susanto</t>
+  </si>
+  <si>
+    <t>Muhammad Ibrahim</t>
+  </si>
+  <si>
+    <t>Surra Arjun</t>
+  </si>
+  <si>
+    <t>Andri Kurniawan Adrianto</t>
+  </si>
+  <si>
     <t>Abdoni Adhi Prakoso</t>
   </si>
   <si>
-    <t>Adam Kurniawan Takariyanto</t>
-  </si>
-  <si>
-    <t>Adi Gunawan</t>
-  </si>
-  <si>
-    <t>Adil Syaifullah</t>
-  </si>
-  <si>
-    <t>Andri Kurniawan Adrianto</t>
-  </si>
-  <si>
-    <t>Brigitta D Avriella</t>
-  </si>
-  <si>
-    <t>Esa Ubadi Taqwa</t>
-  </si>
-  <si>
-    <t>Hendro Susanto</t>
-  </si>
-  <si>
-    <t>M. Usman Fauzi</t>
-  </si>
-  <si>
-    <t>Muhammad Ibrahim</t>
-  </si>
-  <si>
-    <t>Muhammad Reza Pratama</t>
-  </si>
-  <si>
-    <t>Mujab Fahmi</t>
-  </si>
-  <si>
-    <t>Surra Arjun</t>
-  </si>
-  <si>
-    <t>Jodi Juliansah</t>
+    <t>Fandika Saputra</t>
+  </si>
+  <si>
+    <t>Michael Christian</t>
   </si>
 </sst>
 </file>
@@ -415,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +421,7 @@
         <v>4001598</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,44 +429,44 @@
         <v>4001581</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4001132</v>
+        <v>4001385</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4000952</v>
+        <v>4001570</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4001385</v>
+        <v>4001526</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4001344</v>
+        <v>4001119</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>4001200</v>
+        <v>4001572</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -492,58 +474,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4001570</v>
+        <v>4001665</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>4001399</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>4001526</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4001208</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>4001632</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>4001119</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>4001441</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing New Build with user profile
</commit_message>
<xml_diff>
--- a/coba.xlsx
+++ b/coba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RnD\auto-fill-ms-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5FEB69-F476-4021-8F1F-8406759BE4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59968D10-7E6E-491C-996F-349B3B2798B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>NIK</t>
   </si>
@@ -51,17 +51,20 @@
     <t>Abdoni Adhi Prakoso</t>
   </si>
   <si>
-    <t>Fandika Saputra</t>
-  </si>
-  <si>
     <t>Michael Christian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Susetyadi TP </t>
+  </si>
+  <si>
+    <t>Brigitta d'Avriella</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +80,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -113,10 +129,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,11 +483,11 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>4001572</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
+      <c r="A8" s="3">
+        <v>4000224</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,7 +495,15 @@
         <v>4001665</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>4001344</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>